<commit_message>
Added medicals taking for subjects to keep GPA
</commit_message>
<xml_diff>
--- a/data/summary/GPA_Summary.xlsx
+++ b/data/summary/GPA_Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H221"/>
+  <dimension ref="A1:I221"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>TotalMC</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,6 +507,9 @@
       <c r="H2" t="n">
         <v>0</v>
       </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -530,6 +538,9 @@
       <c r="H3" t="n">
         <v>0</v>
       </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -558,6 +569,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
+      <c r="I4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -586,6 +600,9 @@
       <c r="H5" t="n">
         <v>0</v>
       </c>
+      <c r="I5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -614,6 +631,9 @@
       <c r="H6" t="n">
         <v>0</v>
       </c>
+      <c r="I6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -642,6 +662,9 @@
       <c r="H7" t="n">
         <v>0</v>
       </c>
+      <c r="I7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -670,6 +693,9 @@
       <c r="H8" t="n">
         <v>0</v>
       </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -698,6 +724,9 @@
       <c r="H9" t="n">
         <v>0</v>
       </c>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -726,6 +755,9 @@
       <c r="H10" t="n">
         <v>0</v>
       </c>
+      <c r="I10" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -754,6 +786,9 @@
       <c r="H11" t="n">
         <v>0</v>
       </c>
+      <c r="I11" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -782,6 +817,9 @@
       <c r="H12" t="n">
         <v>0</v>
       </c>
+      <c r="I12" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -810,6 +848,9 @@
       <c r="H13" t="n">
         <v>0</v>
       </c>
+      <c r="I13" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -838,6 +879,9 @@
       <c r="H14" t="n">
         <v>0</v>
       </c>
+      <c r="I14" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -866,6 +910,9 @@
       <c r="H15" t="n">
         <v>0</v>
       </c>
+      <c r="I15" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -894,6 +941,9 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -922,6 +972,9 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
+      <c r="I17" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -950,6 +1003,9 @@
       <c r="H18" t="n">
         <v>0</v>
       </c>
+      <c r="I18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -978,6 +1034,9 @@
       <c r="H19" t="n">
         <v>0</v>
       </c>
+      <c r="I19" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1006,6 +1065,9 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
+      <c r="I20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1034,6 +1096,9 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1062,6 +1127,9 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1090,6 +1158,9 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1118,6 +1189,9 @@
       <c r="H24" t="n">
         <v>0</v>
       </c>
+      <c r="I24" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1146,6 +1220,9 @@
       <c r="H25" t="n">
         <v>5</v>
       </c>
+      <c r="I25" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1174,6 +1251,9 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1202,6 +1282,9 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1230,6 +1313,9 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1258,6 +1344,9 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
+      <c r="I29" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1286,6 +1375,9 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
+      <c r="I30" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1314,6 +1406,9 @@
       <c r="H31" t="n">
         <v>0</v>
       </c>
+      <c r="I31" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1342,6 +1437,9 @@
       <c r="H32" t="n">
         <v>0</v>
       </c>
+      <c r="I32" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1370,6 +1468,9 @@
       <c r="H33" t="n">
         <v>0</v>
       </c>
+      <c r="I33" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1398,6 +1499,9 @@
       <c r="H34" t="n">
         <v>0</v>
       </c>
+      <c r="I34" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1426,6 +1530,9 @@
       <c r="H35" t="n">
         <v>0</v>
       </c>
+      <c r="I35" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1454,6 +1561,9 @@
       <c r="H36" t="n">
         <v>2</v>
       </c>
+      <c r="I36" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1482,6 +1592,9 @@
       <c r="H37" t="n">
         <v>0</v>
       </c>
+      <c r="I37" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1510,6 +1623,9 @@
       <c r="H38" t="n">
         <v>2</v>
       </c>
+      <c r="I38" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1538,6 +1654,9 @@
       <c r="H39" t="n">
         <v>0</v>
       </c>
+      <c r="I39" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1566,6 +1685,9 @@
       <c r="H40" t="n">
         <v>0</v>
       </c>
+      <c r="I40" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1594,6 +1716,9 @@
       <c r="H41" t="n">
         <v>0</v>
       </c>
+      <c r="I41" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1622,6 +1747,9 @@
       <c r="H42" t="n">
         <v>3</v>
       </c>
+      <c r="I42" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1650,6 +1778,9 @@
       <c r="H43" t="n">
         <v>0</v>
       </c>
+      <c r="I43" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1678,6 +1809,9 @@
       <c r="H44" t="n">
         <v>0</v>
       </c>
+      <c r="I44" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1706,6 +1840,9 @@
       <c r="H45" t="n">
         <v>0</v>
       </c>
+      <c r="I45" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1734,6 +1871,9 @@
       <c r="H46" t="n">
         <v>3</v>
       </c>
+      <c r="I46" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1762,6 +1902,9 @@
       <c r="H47" t="n">
         <v>0</v>
       </c>
+      <c r="I47" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1790,6 +1933,9 @@
       <c r="H48" t="n">
         <v>2</v>
       </c>
+      <c r="I48" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1818,6 +1964,9 @@
       <c r="H49" t="n">
         <v>0</v>
       </c>
+      <c r="I49" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1846,6 +1995,9 @@
       <c r="H50" t="n">
         <v>0</v>
       </c>
+      <c r="I50" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1874,6 +2026,9 @@
       <c r="H51" t="n">
         <v>0</v>
       </c>
+      <c r="I51" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1902,6 +2057,9 @@
       <c r="H52" t="n">
         <v>0</v>
       </c>
+      <c r="I52" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1930,6 +2088,9 @@
       <c r="H53" t="n">
         <v>0</v>
       </c>
+      <c r="I53" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1958,6 +2119,9 @@
       <c r="H54" t="n">
         <v>0</v>
       </c>
+      <c r="I54" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1986,6 +2150,9 @@
       <c r="H55" t="n">
         <v>0</v>
       </c>
+      <c r="I55" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2014,6 +2181,9 @@
       <c r="H56" t="n">
         <v>3</v>
       </c>
+      <c r="I56" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2042,6 +2212,9 @@
       <c r="H57" t="n">
         <v>0</v>
       </c>
+      <c r="I57" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2070,6 +2243,9 @@
       <c r="H58" t="n">
         <v>0</v>
       </c>
+      <c r="I58" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2098,6 +2274,9 @@
       <c r="H59" t="n">
         <v>0</v>
       </c>
+      <c r="I59" t="n">
+        <v>58</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2126,6 +2305,9 @@
       <c r="H60" t="n">
         <v>0</v>
       </c>
+      <c r="I60" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2154,6 +2336,9 @@
       <c r="H61" t="n">
         <v>0</v>
       </c>
+      <c r="I61" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2182,6 +2367,9 @@
       <c r="H62" t="n">
         <v>0</v>
       </c>
+      <c r="I62" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2210,6 +2398,9 @@
       <c r="H63" t="n">
         <v>0</v>
       </c>
+      <c r="I63" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2238,6 +2429,9 @@
       <c r="H64" t="n">
         <v>0</v>
       </c>
+      <c r="I64" t="n">
+        <v>63</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2266,6 +2460,9 @@
       <c r="H65" t="n">
         <v>0</v>
       </c>
+      <c r="I65" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2294,6 +2491,9 @@
       <c r="H66" t="n">
         <v>0</v>
       </c>
+      <c r="I66" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2322,6 +2522,9 @@
       <c r="H67" t="n">
         <v>0</v>
       </c>
+      <c r="I67" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2350,6 +2553,9 @@
       <c r="H68" t="n">
         <v>0</v>
       </c>
+      <c r="I68" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2378,6 +2584,9 @@
       <c r="H69" t="n">
         <v>0</v>
       </c>
+      <c r="I69" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2406,6 +2615,9 @@
       <c r="H70" t="n">
         <v>6</v>
       </c>
+      <c r="I70" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2434,6 +2646,9 @@
       <c r="H71" t="n">
         <v>0</v>
       </c>
+      <c r="I71" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2462,6 +2677,9 @@
       <c r="H72" t="n">
         <v>0</v>
       </c>
+      <c r="I72" t="n">
+        <v>71</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2490,6 +2708,9 @@
       <c r="H73" t="n">
         <v>0</v>
       </c>
+      <c r="I73" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2518,6 +2739,9 @@
       <c r="H74" t="n">
         <v>9</v>
       </c>
+      <c r="I74" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2546,6 +2770,9 @@
       <c r="H75" t="n">
         <v>0</v>
       </c>
+      <c r="I75" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2574,6 +2801,9 @@
       <c r="H76" t="n">
         <v>3</v>
       </c>
+      <c r="I76" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2602,6 +2832,9 @@
       <c r="H77" t="n">
         <v>0</v>
       </c>
+      <c r="I77" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2630,6 +2863,9 @@
       <c r="H78" t="n">
         <v>0</v>
       </c>
+      <c r="I78" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2658,6 +2894,9 @@
       <c r="H79" t="n">
         <v>2</v>
       </c>
+      <c r="I79" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2686,6 +2925,9 @@
       <c r="H80" t="n">
         <v>0</v>
       </c>
+      <c r="I80" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2714,6 +2956,9 @@
       <c r="H81" t="n">
         <v>0</v>
       </c>
+      <c r="I81" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2742,6 +2987,9 @@
       <c r="H82" t="n">
         <v>0</v>
       </c>
+      <c r="I82" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2770,6 +3018,9 @@
       <c r="H83" t="n">
         <v>0</v>
       </c>
+      <c r="I83" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2798,6 +3049,9 @@
       <c r="H84" t="n">
         <v>2</v>
       </c>
+      <c r="I84" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2826,6 +3080,9 @@
       <c r="H85" t="n">
         <v>3</v>
       </c>
+      <c r="I85" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2854,6 +3111,9 @@
       <c r="H86" t="n">
         <v>2</v>
       </c>
+      <c r="I86" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2882,6 +3142,9 @@
       <c r="H87" t="n">
         <v>0</v>
       </c>
+      <c r="I87" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2910,6 +3173,9 @@
       <c r="H88" t="n">
         <v>4</v>
       </c>
+      <c r="I88" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2938,6 +3204,9 @@
       <c r="H89" t="n">
         <v>0</v>
       </c>
+      <c r="I89" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2966,6 +3235,9 @@
       <c r="H90" t="n">
         <v>0</v>
       </c>
+      <c r="I90" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2994,6 +3266,9 @@
       <c r="H91" t="n">
         <v>2</v>
       </c>
+      <c r="I91" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3022,6 +3297,9 @@
       <c r="H92" t="n">
         <v>0</v>
       </c>
+      <c r="I92" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3050,6 +3328,9 @@
       <c r="H93" t="n">
         <v>0</v>
       </c>
+      <c r="I93" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3078,6 +3359,9 @@
       <c r="H94" t="n">
         <v>0</v>
       </c>
+      <c r="I94" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3106,6 +3390,9 @@
       <c r="H95" t="n">
         <v>0</v>
       </c>
+      <c r="I95" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3134,6 +3421,9 @@
       <c r="H96" t="n">
         <v>0</v>
       </c>
+      <c r="I96" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3162,6 +3452,9 @@
       <c r="H97" t="n">
         <v>0</v>
       </c>
+      <c r="I97" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3190,6 +3483,9 @@
       <c r="H98" t="n">
         <v>0</v>
       </c>
+      <c r="I98" t="n">
+        <v>97</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3218,6 +3514,9 @@
       <c r="H99" t="n">
         <v>0</v>
       </c>
+      <c r="I99" t="n">
+        <v>98</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3246,6 +3545,9 @@
       <c r="H100" t="n">
         <v>0</v>
       </c>
+      <c r="I100" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3274,6 +3576,9 @@
       <c r="H101" t="n">
         <v>0</v>
       </c>
+      <c r="I101" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3302,6 +3607,9 @@
       <c r="H102" t="n">
         <v>0</v>
       </c>
+      <c r="I102" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3330,6 +3638,9 @@
       <c r="H103" t="n">
         <v>0</v>
       </c>
+      <c r="I103" t="n">
+        <v>102</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3358,6 +3669,9 @@
       <c r="H104" t="n">
         <v>0</v>
       </c>
+      <c r="I104" t="n">
+        <v>103</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3386,6 +3700,9 @@
       <c r="H105" t="n">
         <v>0</v>
       </c>
+      <c r="I105" t="n">
+        <v>104</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3414,6 +3731,9 @@
       <c r="H106" t="n">
         <v>4</v>
       </c>
+      <c r="I106" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3442,6 +3762,9 @@
       <c r="H107" t="n">
         <v>0</v>
       </c>
+      <c r="I107" t="n">
+        <v>106</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3470,6 +3793,9 @@
       <c r="H108" t="n">
         <v>0</v>
       </c>
+      <c r="I108" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3498,6 +3824,9 @@
       <c r="H109" t="n">
         <v>6</v>
       </c>
+      <c r="I109" t="n">
+        <v>108</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3526,6 +3855,9 @@
       <c r="H110" t="n">
         <v>0</v>
       </c>
+      <c r="I110" t="n">
+        <v>109</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3554,6 +3886,9 @@
       <c r="H111" t="n">
         <v>0</v>
       </c>
+      <c r="I111" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3582,6 +3917,9 @@
       <c r="H112" t="n">
         <v>0</v>
       </c>
+      <c r="I112" t="n">
+        <v>111</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3610,6 +3948,9 @@
       <c r="H113" t="n">
         <v>9</v>
       </c>
+      <c r="I113" t="n">
+        <v>112</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3638,6 +3979,9 @@
       <c r="H114" t="n">
         <v>9</v>
       </c>
+      <c r="I114" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3666,6 +4010,9 @@
       <c r="H115" t="n">
         <v>9</v>
       </c>
+      <c r="I115" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3694,6 +4041,9 @@
       <c r="H116" t="n">
         <v>4</v>
       </c>
+      <c r="I116" t="n">
+        <v>115</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3722,6 +4072,9 @@
       <c r="H117" t="n">
         <v>0</v>
       </c>
+      <c r="I117" t="n">
+        <v>116</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3750,6 +4103,9 @@
       <c r="H118" t="n">
         <v>0</v>
       </c>
+      <c r="I118" t="n">
+        <v>117</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3778,6 +4134,9 @@
       <c r="H119" t="n">
         <v>24</v>
       </c>
+      <c r="I119" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3806,6 +4165,9 @@
       <c r="H120" t="n">
         <v>5</v>
       </c>
+      <c r="I120" t="n">
+        <v>119</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3834,6 +4196,9 @@
       <c r="H121" t="n">
         <v>12</v>
       </c>
+      <c r="I121" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3862,6 +4227,9 @@
       <c r="H122" t="n">
         <v>0</v>
       </c>
+      <c r="I122" t="n">
+        <v>121</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3890,6 +4258,9 @@
       <c r="H123" t="n">
         <v>0</v>
       </c>
+      <c r="I123" t="n">
+        <v>122</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3918,6 +4289,9 @@
       <c r="H124" t="n">
         <v>2</v>
       </c>
+      <c r="I124" t="n">
+        <v>123</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3946,6 +4320,9 @@
       <c r="H125" t="n">
         <v>4</v>
       </c>
+      <c r="I125" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3974,6 +4351,9 @@
       <c r="H126" t="n">
         <v>0</v>
       </c>
+      <c r="I126" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4002,6 +4382,9 @@
       <c r="H127" t="n">
         <v>3</v>
       </c>
+      <c r="I127" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4030,6 +4413,9 @@
       <c r="H128" t="n">
         <v>3</v>
       </c>
+      <c r="I128" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4058,6 +4444,9 @@
       <c r="H129" t="n">
         <v>0</v>
       </c>
+      <c r="I129" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4086,6 +4475,9 @@
       <c r="H130" t="n">
         <v>0</v>
       </c>
+      <c r="I130" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4114,6 +4506,9 @@
       <c r="H131" t="n">
         <v>0</v>
       </c>
+      <c r="I131" t="n">
+        <v>130</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4142,6 +4537,9 @@
       <c r="H132" t="n">
         <v>0</v>
       </c>
+      <c r="I132" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4170,6 +4568,9 @@
       <c r="H133" t="n">
         <v>0</v>
       </c>
+      <c r="I133" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4198,6 +4599,9 @@
       <c r="H134" t="n">
         <v>0</v>
       </c>
+      <c r="I134" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4226,6 +4630,9 @@
       <c r="H135" t="n">
         <v>0</v>
       </c>
+      <c r="I135" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4254,6 +4661,9 @@
       <c r="H136" t="n">
         <v>2</v>
       </c>
+      <c r="I136" t="n">
+        <v>135</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4282,6 +4692,9 @@
       <c r="H137" t="n">
         <v>11</v>
       </c>
+      <c r="I137" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4310,6 +4723,9 @@
       <c r="H138" t="n">
         <v>1</v>
       </c>
+      <c r="I138" t="n">
+        <v>137</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4338,6 +4754,9 @@
       <c r="H139" t="n">
         <v>2</v>
       </c>
+      <c r="I139" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4366,6 +4785,9 @@
       <c r="H140" t="n">
         <v>17</v>
       </c>
+      <c r="I140" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4394,6 +4816,9 @@
       <c r="H141" t="n">
         <v>0</v>
       </c>
+      <c r="I141" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4422,6 +4847,9 @@
       <c r="H142" t="n">
         <v>18</v>
       </c>
+      <c r="I142" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4450,6 +4878,9 @@
       <c r="H143" t="n">
         <v>7</v>
       </c>
+      <c r="I143" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4478,6 +4909,9 @@
       <c r="H144" t="n">
         <v>2</v>
       </c>
+      <c r="I144" t="n">
+        <v>143</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4506,6 +4940,9 @@
       <c r="H145" t="n">
         <v>0</v>
       </c>
+      <c r="I145" t="n">
+        <v>144</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4534,6 +4971,9 @@
       <c r="H146" t="n">
         <v>0</v>
       </c>
+      <c r="I146" t="n">
+        <v>145</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4562,6 +5002,9 @@
       <c r="H147" t="n">
         <v>7</v>
       </c>
+      <c r="I147" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4590,6 +5033,9 @@
       <c r="H148" t="n">
         <v>19</v>
       </c>
+      <c r="I148" t="n">
+        <v>147</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4618,6 +5064,9 @@
       <c r="H149" t="n">
         <v>2</v>
       </c>
+      <c r="I149" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4646,6 +5095,9 @@
       <c r="H150" t="n">
         <v>6</v>
       </c>
+      <c r="I150" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -4674,6 +5126,9 @@
       <c r="H151" t="n">
         <v>0</v>
       </c>
+      <c r="I151" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -4702,6 +5157,9 @@
       <c r="H152" t="n">
         <v>0</v>
       </c>
+      <c r="I152" t="n">
+        <v>151</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -4730,6 +5188,9 @@
       <c r="H153" t="n">
         <v>0</v>
       </c>
+      <c r="I153" t="n">
+        <v>152</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -4758,6 +5219,9 @@
       <c r="H154" t="n">
         <v>0</v>
       </c>
+      <c r="I154" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -4786,6 +5250,9 @@
       <c r="H155" t="n">
         <v>7</v>
       </c>
+      <c r="I155" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -4814,6 +5281,9 @@
       <c r="H156" t="n">
         <v>0</v>
       </c>
+      <c r="I156" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -4842,6 +5312,9 @@
       <c r="H157" t="n">
         <v>0</v>
       </c>
+      <c r="I157" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -4870,6 +5343,9 @@
       <c r="H158" t="n">
         <v>5</v>
       </c>
+      <c r="I158" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -4898,6 +5374,9 @@
       <c r="H159" t="n">
         <v>0</v>
       </c>
+      <c r="I159" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -4926,6 +5405,9 @@
       <c r="H160" t="n">
         <v>0</v>
       </c>
+      <c r="I160" t="n">
+        <v>159</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -4954,6 +5436,9 @@
       <c r="H161" t="n">
         <v>2</v>
       </c>
+      <c r="I161" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -4982,6 +5467,9 @@
       <c r="H162" t="n">
         <v>0</v>
       </c>
+      <c r="I162" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5010,6 +5498,9 @@
       <c r="H163" t="n">
         <v>2</v>
       </c>
+      <c r="I163" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5038,6 +5529,9 @@
       <c r="H164" t="n">
         <v>9</v>
       </c>
+      <c r="I164" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5066,6 +5560,9 @@
       <c r="H165" t="n">
         <v>0</v>
       </c>
+      <c r="I165" t="n">
+        <v>164</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5094,6 +5591,9 @@
       <c r="H166" t="n">
         <v>0</v>
       </c>
+      <c r="I166" t="n">
+        <v>165</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5122,6 +5622,9 @@
       <c r="H167" t="n">
         <v>3</v>
       </c>
+      <c r="I167" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5150,6 +5653,9 @@
       <c r="H168" t="n">
         <v>3</v>
       </c>
+      <c r="I168" t="n">
+        <v>167</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5178,6 +5684,9 @@
       <c r="H169" t="n">
         <v>8</v>
       </c>
+      <c r="I169" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5206,6 +5715,9 @@
       <c r="H170" t="n">
         <v>23</v>
       </c>
+      <c r="I170" t="n">
+        <v>169</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -5234,6 +5746,9 @@
       <c r="H171" t="n">
         <v>32</v>
       </c>
+      <c r="I171" t="n">
+        <v>170</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5262,6 +5777,9 @@
       <c r="H172" t="n">
         <v>0</v>
       </c>
+      <c r="I172" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5290,6 +5808,9 @@
       <c r="H173" t="n">
         <v>0</v>
       </c>
+      <c r="I173" t="n">
+        <v>172</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -5318,6 +5839,9 @@
       <c r="H174" t="n">
         <v>16</v>
       </c>
+      <c r="I174" t="n">
+        <v>173</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -5346,6 +5870,9 @@
       <c r="H175" t="n">
         <v>0</v>
       </c>
+      <c r="I175" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -5374,6 +5901,9 @@
       <c r="H176" t="n">
         <v>0</v>
       </c>
+      <c r="I176" t="n">
+        <v>175</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -5402,6 +5932,9 @@
       <c r="H177" t="n">
         <v>9</v>
       </c>
+      <c r="I177" t="n">
+        <v>176</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -5430,6 +5963,9 @@
       <c r="H178" t="n">
         <v>4</v>
       </c>
+      <c r="I178" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -5458,6 +5994,9 @@
       <c r="H179" t="n">
         <v>6</v>
       </c>
+      <c r="I179" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -5486,6 +6025,9 @@
       <c r="H180" t="n">
         <v>10</v>
       </c>
+      <c r="I180" t="n">
+        <v>179</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -5514,6 +6056,9 @@
       <c r="H181" t="n">
         <v>0</v>
       </c>
+      <c r="I181" t="n">
+        <v>180</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5542,6 +6087,9 @@
       <c r="H182" t="n">
         <v>11</v>
       </c>
+      <c r="I182" t="n">
+        <v>181</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -5570,6 +6118,9 @@
       <c r="H183" t="n">
         <v>0</v>
       </c>
+      <c r="I183" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -5598,6 +6149,9 @@
       <c r="H184" t="n">
         <v>2</v>
       </c>
+      <c r="I184" t="n">
+        <v>183</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -5626,6 +6180,9 @@
       <c r="H185" t="n">
         <v>24</v>
       </c>
+      <c r="I185" t="n">
+        <v>184</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -5654,6 +6211,9 @@
       <c r="H186" t="n">
         <v>27</v>
       </c>
+      <c r="I186" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -5682,6 +6242,9 @@
       <c r="H187" t="n">
         <v>18</v>
       </c>
+      <c r="I187" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -5710,6 +6273,9 @@
       <c r="H188" t="n">
         <v>23</v>
       </c>
+      <c r="I188" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -5738,6 +6304,9 @@
       <c r="H189" t="n">
         <v>0</v>
       </c>
+      <c r="I189" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -5766,6 +6335,9 @@
       <c r="H190" t="n">
         <v>3</v>
       </c>
+      <c r="I190" t="n">
+        <v>189</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -5794,6 +6366,9 @@
       <c r="H191" t="n">
         <v>6</v>
       </c>
+      <c r="I191" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -5822,6 +6397,9 @@
       <c r="H192" t="n">
         <v>2</v>
       </c>
+      <c r="I192" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -5850,6 +6428,9 @@
       <c r="H193" t="n">
         <v>7</v>
       </c>
+      <c r="I193" t="n">
+        <v>192</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -5878,6 +6459,9 @@
       <c r="H194" t="n">
         <v>15</v>
       </c>
+      <c r="I194" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -5906,6 +6490,9 @@
       <c r="H195" t="n">
         <v>28</v>
       </c>
+      <c r="I195" t="n">
+        <v>194</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -5934,6 +6521,9 @@
       <c r="H196" t="n">
         <v>19</v>
       </c>
+      <c r="I196" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -5962,6 +6552,9 @@
       <c r="H197" t="n">
         <v>3</v>
       </c>
+      <c r="I197" t="n">
+        <v>196</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -5990,6 +6583,9 @@
       <c r="H198" t="n">
         <v>5</v>
       </c>
+      <c r="I198" t="n">
+        <v>197</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6018,6 +6614,9 @@
       <c r="H199" t="n">
         <v>0</v>
       </c>
+      <c r="I199" t="n">
+        <v>198</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6046,6 +6645,9 @@
       <c r="H200" t="n">
         <v>6</v>
       </c>
+      <c r="I200" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -6074,6 +6676,9 @@
       <c r="H201" t="n">
         <v>9</v>
       </c>
+      <c r="I201" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -6102,6 +6707,9 @@
       <c r="H202" t="n">
         <v>19</v>
       </c>
+      <c r="I202" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -6130,6 +6738,9 @@
       <c r="H203" t="n">
         <v>9</v>
       </c>
+      <c r="I203" t="n">
+        <v>202</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -6158,6 +6769,9 @@
       <c r="H204" t="n">
         <v>15</v>
       </c>
+      <c r="I204" t="n">
+        <v>203</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -6186,6 +6800,9 @@
       <c r="H205" t="n">
         <v>3</v>
       </c>
+      <c r="I205" t="n">
+        <v>204</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -6214,6 +6831,9 @@
       <c r="H206" t="n">
         <v>12</v>
       </c>
+      <c r="I206" t="n">
+        <v>205</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -6242,6 +6862,9 @@
       <c r="H207" t="n">
         <v>0</v>
       </c>
+      <c r="I207" t="n">
+        <v>206</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -6270,6 +6893,9 @@
       <c r="H208" t="n">
         <v>0</v>
       </c>
+      <c r="I208" t="n">
+        <v>207</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6298,6 +6924,9 @@
       <c r="H209" t="n">
         <v>7</v>
       </c>
+      <c r="I209" t="n">
+        <v>208</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -6326,6 +6955,9 @@
       <c r="H210" t="n">
         <v>2</v>
       </c>
+      <c r="I210" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -6354,6 +6986,9 @@
       <c r="H211" t="n">
         <v>2</v>
       </c>
+      <c r="I211" t="n">
+        <v>210</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -6382,6 +7017,9 @@
       <c r="H212" t="n">
         <v>27</v>
       </c>
+      <c r="I212" t="n">
+        <v>211</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -6410,6 +7048,9 @@
       <c r="H213" t="n">
         <v>11</v>
       </c>
+      <c r="I213" t="n">
+        <v>212</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -6438,6 +7079,9 @@
       <c r="H214" t="n">
         <v>3</v>
       </c>
+      <c r="I214" t="n">
+        <v>213</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -6466,6 +7110,9 @@
       <c r="H215" t="n">
         <v>30</v>
       </c>
+      <c r="I215" t="n">
+        <v>214</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -6494,6 +7141,9 @@
       <c r="H216" t="n">
         <v>32</v>
       </c>
+      <c r="I216" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -6522,6 +7172,9 @@
       <c r="H217" t="n">
         <v>18</v>
       </c>
+      <c r="I217" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -6550,6 +7203,9 @@
       <c r="H218" t="n">
         <v>26</v>
       </c>
+      <c r="I218" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -6578,6 +7234,9 @@
       <c r="H219" t="n">
         <v>8</v>
       </c>
+      <c r="I219" t="n">
+        <v>218</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -6606,6 +7265,9 @@
       <c r="H220" t="n">
         <v>0</v>
       </c>
+      <c r="I220" t="n">
+        <v>219</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -6633,6 +7295,9 @@
       </c>
       <c r="H221" t="n">
         <v>5</v>
+      </c>
+      <c r="I221" t="n">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>